<commit_message>
Temporal files and file chooser modifications
</commit_message>
<xml_diff>
--- a/data/output/output9.xlsx
+++ b/data/output/output9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\GitHub\ExcelDataProcessing\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D96955D-DB99-4563-BA8F-1D8C803EFAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5428B3-45A3-414A-8D3F-AB518B18D7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -103,9 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,36 +129,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -183,289 +157,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,415 +513,415 @@
       </c>
     </row>
     <row r="2" ht="14.4" customHeight="true">
-      <c r="A2" t="n" s="35">
+      <c r="A2" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B2" t="s" s="23">
+      <c r="B2" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C2" t="s" s="24">
+      <c r="C2" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D2" t="n" s="24">
+      <c r="D2" t="n" s="1">
         <v>6.0</v>
       </c>
-      <c r="E2" t="n" s="24">
+      <c r="E2" t="n" s="1">
         <v>15.0</v>
       </c>
-      <c r="F2" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G2" t="n" s="45">
+      <c r="F2" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G2" t="n" s="1">
         <v>3.9</v>
       </c>
-      <c r="H2" t="n" s="25">
+      <c r="H2" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I2" t="n" s="26">
+      <c r="I2" t="n" s="1">
         <v>189.0</v>
       </c>
-      <c r="J2" t="n" s="26">
+      <c r="J2" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K2" t="n" s="26">
+      <c r="K2" t="n" s="1">
         <v>222.0</v>
       </c>
-      <c r="L2" t="n" s="26">
+      <c r="L2" t="n" s="1">
         <v>1634.0</v>
       </c>
-      <c r="M2" t="n" s="26">
+      <c r="M2" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N2" t="n" s="24">
+      <c r="N2" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O2" t="n" s="26">
+      <c r="O2" t="n" s="1">
         <v>1947.0</v>
       </c>
-      <c r="P2" t="n" s="24">
+      <c r="P2" t="n" s="1">
         <v>11.0</v>
       </c>
-      <c r="Q2" t="n" s="24">
+      <c r="Q2" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R2" t="n" s="24">
+      <c r="R2" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S2" t="n" s="36">
+      <c r="S2" t="n" s="1">
         <v>12522.828213005983</v>
       </c>
     </row>
     <row r="3" ht="14.4" customHeight="true">
-      <c r="A3" t="n" s="35">
+      <c r="A3" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B3" t="s" s="23">
+      <c r="B3" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C3" t="s" s="24">
+      <c r="C3" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D3" t="n" s="24">
+      <c r="D3" t="n" s="1">
         <v>7.0</v>
       </c>
-      <c r="E3" t="n" s="24">
+      <c r="E3" t="n" s="1">
         <v>16.0</v>
       </c>
-      <c r="F3" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G3" t="n" s="45">
+      <c r="F3" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G3" t="n" s="1">
         <v>3.9</v>
       </c>
-      <c r="H3" t="n" s="25">
+      <c r="H3" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I3" t="n" s="26">
+      <c r="I3" t="n" s="1">
         <v>194.0</v>
       </c>
-      <c r="J3" t="n" s="26">
+      <c r="J3" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K3" t="n" s="26">
+      <c r="K3" t="n" s="1">
         <v>222.0</v>
       </c>
-      <c r="L3" t="n" s="26">
+      <c r="L3" t="n" s="1">
         <v>1679.0</v>
       </c>
-      <c r="M3" t="n" s="26">
+      <c r="M3" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N3" t="n" s="24">
+      <c r="N3" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O3" t="n" s="26">
+      <c r="O3" t="n" s="1">
         <v>1947.0</v>
       </c>
-      <c r="P3" t="n" s="24">
+      <c r="P3" t="n" s="1">
         <v>11.0</v>
       </c>
-      <c r="Q3" t="n" s="24">
+      <c r="Q3" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R3" t="n" s="24">
+      <c r="R3" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S3" t="n" s="36">
+      <c r="S3" t="n" s="1">
         <v>12116.616161880596</v>
       </c>
     </row>
     <row r="4" ht="14.4" customHeight="true">
-      <c r="A4" t="n" s="35">
+      <c r="A4" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B4" t="s" s="23">
+      <c r="B4" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C4" t="s" s="24">
+      <c r="C4" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D4" t="n" s="24">
+      <c r="D4" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="E4" t="n" s="24">
+      <c r="E4" t="n" s="1">
         <v>17.0</v>
       </c>
-      <c r="F4" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G4" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="H4" t="n" s="25">
+      <c r="F4" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G4" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="H4" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I4" t="n" s="26">
+      <c r="I4" t="n" s="1">
         <v>217.0</v>
       </c>
-      <c r="J4" t="n" s="26">
+      <c r="J4" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K4" t="n" s="26">
+      <c r="K4" t="n" s="1">
         <v>234.0</v>
       </c>
-      <c r="L4" t="n" s="26">
+      <c r="L4" t="n" s="1">
         <v>1897.0</v>
       </c>
-      <c r="M4" t="n" s="26">
+      <c r="M4" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N4" t="n" s="24">
+      <c r="N4" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O4" t="n" s="26">
+      <c r="O4" t="n" s="1">
         <v>2055.0</v>
       </c>
-      <c r="P4" t="n" s="24">
+      <c r="P4" t="n" s="1">
         <v>26.0</v>
       </c>
-      <c r="Q4" t="n" s="24">
+      <c r="Q4" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R4" t="n" s="24">
+      <c r="R4" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S4" t="n" s="36">
+      <c r="S4" t="n" s="1">
         <v>10501.343345103818</v>
       </c>
     </row>
     <row r="5" ht="14.4" customHeight="true">
-      <c r="A5" t="n" s="35">
+      <c r="A5" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B5" t="s" s="23">
+      <c r="B5" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C5" t="s" s="24">
+      <c r="C5" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D5" t="n" s="24">
+      <c r="D5" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="E5" t="n" s="24">
+      <c r="E5" t="n" s="1">
         <v>18.0</v>
       </c>
-      <c r="F5" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G5" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="H5" t="n" s="25">
+      <c r="F5" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G5" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="H5" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I5" t="n" s="26">
+      <c r="I5" t="n" s="1">
         <v>219.0</v>
       </c>
-      <c r="J5" t="n" s="26">
+      <c r="J5" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K5" t="n" s="26">
+      <c r="K5" t="n" s="1">
         <v>234.0</v>
       </c>
-      <c r="L5" t="n" s="26">
+      <c r="L5" t="n" s="1">
         <v>1917.0</v>
       </c>
-      <c r="M5" t="n" s="26">
+      <c r="M5" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N5" t="n" s="24">
+      <c r="N5" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O5" t="n" s="26">
+      <c r="O5" t="n" s="1">
         <v>2055.0</v>
       </c>
-      <c r="P5" t="n" s="24">
+      <c r="P5" t="n" s="1">
         <v>26.0</v>
       </c>
-      <c r="Q5" t="n" s="24">
+      <c r="Q5" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R5" t="n" s="24">
+      <c r="R5" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S5" t="n" s="36">
+      <c r="S5" t="n" s="1">
         <v>10377.988444334884</v>
       </c>
     </row>
     <row r="6" ht="14.4" customHeight="true">
-      <c r="A6" t="n" s="35">
+      <c r="A6" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B6" t="s" s="23">
+      <c r="B6" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C6" t="s" s="24">
+      <c r="C6" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D6" t="n" s="24">
+      <c r="D6" t="n" s="1">
         <v>9.0</v>
       </c>
-      <c r="E6" t="n" s="24">
+      <c r="E6" t="n" s="1">
         <v>19.0</v>
       </c>
-      <c r="F6" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G6" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="H6" t="n" s="25">
+      <c r="F6" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G6" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="H6" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I6" t="n" s="26">
+      <c r="I6" t="n" s="1">
         <v>224.0</v>
       </c>
-      <c r="J6" t="n" s="26">
+      <c r="J6" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K6" t="n" s="26">
+      <c r="K6" t="n" s="1">
         <v>234.0</v>
       </c>
-      <c r="L6" t="n" s="26">
+      <c r="L6" t="n" s="1">
         <v>1967.0</v>
       </c>
-      <c r="M6" t="n" s="26">
+      <c r="M6" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N6" t="n" s="24">
+      <c r="N6" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O6" t="n" s="26">
+      <c r="O6" t="n" s="1">
         <v>2055.0</v>
       </c>
-      <c r="P6" t="n" s="24">
+      <c r="P6" t="n" s="1">
         <v>26.0</v>
       </c>
-      <c r="Q6" t="n" s="24">
+      <c r="Q6" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R6" t="n" s="24">
+      <c r="R6" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S6" t="n" s="36">
+      <c r="S6" t="n" s="1">
         <v>10080.031996307938</v>
       </c>
     </row>
     <row r="7" ht="14.4" customHeight="true">
-      <c r="A7" t="n" s="35">
+      <c r="A7" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B7" t="s" s="23">
+      <c r="B7" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="24">
+      <c r="C7" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D7" t="n" s="24">
+      <c r="D7" t="n" s="1">
         <v>9.0</v>
       </c>
-      <c r="E7" t="n" s="24">
+      <c r="E7" t="n" s="1">
         <v>20.0</v>
       </c>
-      <c r="F7" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G7" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="H7" t="n" s="25">
+      <c r="F7" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G7" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="H7" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I7" t="n" s="26">
+      <c r="I7" t="n" s="1">
         <v>226.0</v>
       </c>
-      <c r="J7" t="n" s="26">
+      <c r="J7" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K7" t="n" s="26">
+      <c r="K7" t="n" s="1">
         <v>234.0</v>
       </c>
-      <c r="L7" t="n" s="26">
+      <c r="L7" t="n" s="1">
         <v>1985.0</v>
       </c>
-      <c r="M7" t="n" s="26">
+      <c r="M7" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N7" t="n" s="24">
+      <c r="N7" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O7" t="n" s="26">
+      <c r="O7" t="n" s="1">
         <v>2055.0</v>
       </c>
-      <c r="P7" t="n" s="24">
+      <c r="P7" t="n" s="1">
         <v>26.0</v>
       </c>
-      <c r="Q7" t="n" s="24">
+      <c r="Q7" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R7" t="n" s="24">
+      <c r="R7" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S7" t="n" s="36">
+      <c r="S7" t="n" s="1">
         <v>9970.096740349509</v>
       </c>
     </row>
     <row r="8" ht="14.4" customHeight="true">
-      <c r="A8" t="n" s="35">
+      <c r="A8" t="n" s="1">
         <v>43612.0</v>
       </c>
-      <c r="B8" t="s" s="23">
+      <c r="B8" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C8" t="s" s="24">
+      <c r="C8" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="D8" t="n" s="24">
+      <c r="D8" t="n" s="1">
         <v>9.0</v>
       </c>
-      <c r="E8" t="n" s="24">
+      <c r="E8" t="n" s="1">
         <v>21.0</v>
       </c>
-      <c r="F8" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="G8" t="n" s="45">
-        <v>4.9</v>
-      </c>
-      <c r="H8" t="n" s="25">
+      <c r="F8" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="G8" t="n" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="H8" t="n" s="1">
         <v>8.0</v>
       </c>
-      <c r="I8" t="n" s="26">
+      <c r="I8" t="n" s="1">
         <v>227.0</v>
       </c>
-      <c r="J8" t="n" s="26">
+      <c r="J8" t="n" s="1">
         <v>160.0</v>
       </c>
-      <c r="K8" t="n" s="26">
+      <c r="K8" t="n" s="1">
         <v>234.0</v>
       </c>
-      <c r="L8" t="n" s="26">
+      <c r="L8" t="n" s="1">
         <v>1994.0</v>
       </c>
-      <c r="M8" t="n" s="26">
+      <c r="M8" t="n" s="1">
         <v>1368.0</v>
       </c>
-      <c r="N8" t="n" s="24">
+      <c r="N8" t="n" s="1">
         <v>13.0</v>
       </c>
-      <c r="O8" t="n" s="26">
+      <c r="O8" t="n" s="1">
         <v>2055.0</v>
       </c>
-      <c r="P8" t="n" s="24">
+      <c r="P8" t="n" s="1">
         <v>26.0</v>
       </c>
-      <c r="Q8" t="n" s="24">
+      <c r="Q8" t="n" s="1">
         <v>3.5</v>
       </c>
-      <c r="R8" t="n" s="24">
+      <c r="R8" t="n" s="1">
         <v>5.2</v>
       </c>
-      <c r="S8" t="n" s="36">
+      <c r="S8" t="n" s="1">
         <v>9918.00516520619</v>
       </c>
     </row>

</xml_diff>